<commit_message>
testing out different grids
</commit_message>
<xml_diff>
--- a/handwriting_grid_template.xlsx
+++ b/handwriting_grid_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\Desktop\Computer_Vision_Finance_OCR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E69D36D8-10B1-48DC-8E4A-E98A8B7CFB0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72310C9C-E1E7-4DBB-B2E8-A04A589554AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{75D4D9EB-5B72-451C-8BEA-2A264F9DEAC3}"/>
   </bookViews>
@@ -33,6 +33,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -70,16 +74,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="dotted">
+      <left style="hair">
         <color indexed="64"/>
       </left>
-      <right style="dotted">
+      <right style="hair">
         <color indexed="64"/>
       </right>
-      <top style="dotted">
+      <top style="hair">
         <color indexed="64"/>
       </top>
-      <bottom style="dotted">
+      <bottom style="hair">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -408,7 +412,7 @@
   <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:Z36"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="19.7" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>